<commit_message>
FIlled out timeline. Added raid damage to md
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samve\Documents\p4s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FBC49BC-116E-4155-82BC-864BCA76D3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE28217-F00D-4375-8F62-903278B35306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{8D2E3F79-257F-4C06-9363-A85105DAD882}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeline" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Searing Stream</t>
   </si>
@@ -61,6 +61,27 @@
   </si>
   <si>
     <t>Yui</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>SW, DM, Ramp, Obl, TBN</t>
+  </si>
+  <si>
+    <t>Rep, HoL</t>
+  </si>
+  <si>
+    <t>Rep, Dark Mis</t>
+  </si>
+  <si>
+    <t>DM, Ramp, Obl, TBN</t>
+  </si>
+  <si>
+    <t>Bolid</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -121,8 +142,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4888E44-E67D-4C82-B52F-A26D3A065EC9}" name="Table1" displayName="Table1" ref="B1:E17" totalsRowShown="0">
-  <autoFilter ref="B1:E17" xr:uid="{A4888E44-E67D-4C82-B52F-A26D3A065EC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4888E44-E67D-4C82-B52F-A26D3A065EC9}" name="Table1" displayName="Table1" ref="B2:E18" totalsRowShown="0">
+  <autoFilter ref="B2:E18" xr:uid="{A4888E44-E67D-4C82-B52F-A26D3A065EC9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E16E36DE-91D8-474E-8528-AE8A3A403C27}" name="Ability"/>
     <tableColumn id="2" xr3:uid="{03C7FDB5-F71A-47B1-AF3D-C5EBF2AEDFA2}" name="Time" dataDxfId="0"/>
@@ -430,37 +451,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B166EE-DAEA-47B4-B122-2BB0B0D1ECBC}">
-  <dimension ref="B1:E17"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6.9444444444444441E-3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -468,55 +483,76 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>2.4305555555555556E-2</v>
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>4.4444444444444446E-2</v>
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>5.9722222222222225E-2</v>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>8.4722222222222213E-2</v>
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>0.12569444444444444</v>
+        <v>8.4722222222222213E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>0.1361111111111111</v>
+        <v>0.12569444444444444</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>0.15138888888888888</v>
+        <v>0.1361111111111111</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -524,63 +560,98 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>0.16319444444444445</v>
+        <v>0.15138888888888888</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>0.18611111111111112</v>
+        <v>0.16319444444444445</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>0.19791666666666666</v>
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>0.24027777777777778</v>
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>0.25</v>
+        <v>0.24027777777777778</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>0.25625000000000003</v>
+        <v>0.25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
-        <v>0.30069444444444443</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <v>0.25625000000000003</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="1">
+        <v>0.30069444444444443</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
         <v>0.3354166666666667</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>